<commit_message>
added the teachers numbers to the excel files
</commit_message>
<xml_diff>
--- a/public/names.xlsx
+++ b/public/names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Root 2034\Documents\gitRepostiry\tahfezy_project_2025\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3F9D6D-2665-489C-AEE5-51EE50F249E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6941477B-2B68-443F-862A-0E45BBBBBD66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{909453FE-4F6A-4FDA-BCF7-D5A7CD4F37A9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="139">
   <si>
     <t>name</t>
   </si>
@@ -364,6 +364,84 @@
   </si>
   <si>
     <t>055 595 6495</t>
+  </si>
+  <si>
+    <t>عبدالسلام الخليوي</t>
+  </si>
+  <si>
+    <t>055 219 2974</t>
+  </si>
+  <si>
+    <t>الزبير الودعان</t>
+  </si>
+  <si>
+    <t>053 474 1996</t>
+  </si>
+  <si>
+    <t>عبدالله البسام</t>
+  </si>
+  <si>
+    <t>059 941 1606</t>
+  </si>
+  <si>
+    <t>عبدالله الصبي</t>
+  </si>
+  <si>
+    <t>055 448 0798</t>
+  </si>
+  <si>
+    <t>حمزة العمري</t>
+  </si>
+  <si>
+    <t>055 799 8853</t>
+  </si>
+  <si>
+    <t>عبدالله الغفيلي</t>
+  </si>
+  <si>
+    <t>058 210 7350</t>
+  </si>
+  <si>
+    <t>عثمان الرشيد</t>
+  </si>
+  <si>
+    <t>055 450 2650</t>
+  </si>
+  <si>
+    <t>اسامة العامر</t>
+  </si>
+  <si>
+    <t>053 575 9023</t>
+  </si>
+  <si>
+    <t>صالح السحيباني</t>
+  </si>
+  <si>
+    <t>050 828 5787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">زياد العصيمي </t>
+  </si>
+  <si>
+    <t>050 847 6425</t>
+  </si>
+  <si>
+    <t>عمر التويجري</t>
+  </si>
+  <si>
+    <t>050 766 9196</t>
+  </si>
+  <si>
+    <t>راكان الناجي</t>
+  </si>
+  <si>
+    <t>058 190 0510</t>
+  </si>
+  <si>
+    <t>مصعب الصقعبي</t>
+  </si>
+  <si>
+    <t>055 759 8613</t>
   </si>
 </sst>
 </file>
@@ -738,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A15376-C4C0-45CB-9412-32B006207686}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,7 +1416,7 @@
         <v>24</v>
       </c>
       <c r="B54" s="4">
-        <v>966553316521</v>
+        <v>553316521</v>
       </c>
       <c r="C54" t="s">
         <v>60</v>
@@ -1349,9 +1427,152 @@
         <v>23</v>
       </c>
       <c r="B55" s="4">
-        <v>966565132154</v>
+        <v>565132154</v>
       </c>
       <c r="C55" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>121</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>123</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>125</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>129</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C64" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>131</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>133</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C66" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>135</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C67" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>137</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C68" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added two new names
</commit_message>
<xml_diff>
--- a/public/names.xlsx
+++ b/public/names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Root 2034\Documents\gitRepostiry\tahfezy_project_2025\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abukhaled/Documents/Temp/tahfezy_project_2025/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6941477B-2B68-443F-862A-0E45BBBBBD66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04C5602-83CC-1142-9C15-860073564A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{909453FE-4F6A-4FDA-BCF7-D5A7CD4F37A9}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{909453FE-4F6A-4FDA-BCF7-D5A7CD4F37A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="142">
   <si>
     <t>name</t>
   </si>
@@ -442,6 +442,15 @@
   </si>
   <si>
     <t>055 759 8613</t>
+  </si>
+  <si>
+    <t>باسل العنزي</t>
+  </si>
+  <si>
+    <t>البراء السحيباني</t>
+  </si>
+  <si>
+    <t>+966 53 412 8937</t>
   </si>
 </sst>
 </file>
@@ -816,19 +825,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A15376-C4C0-45CB-9412-32B006207686}">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -839,7 +848,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -850,7 +859,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -861,7 +870,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -872,7 +881,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -883,7 +892,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -894,7 +903,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -905,7 +914,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -916,7 +925,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -927,7 +936,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -938,7 +947,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -949,7 +958,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -960,7 +969,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -971,7 +980,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -982,7 +991,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
@@ -993,7 +1002,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -1004,7 +1013,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -1015,7 +1024,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1026,7 +1035,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -1037,7 +1046,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
@@ -1048,7 +1057,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -1059,7 +1068,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>5</v>
       </c>
@@ -1070,7 +1079,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>11</v>
       </c>
@@ -1081,7 +1090,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
@@ -1092,7 +1101,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
@@ -1103,7 +1112,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>8</v>
       </c>
@@ -1114,7 +1123,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
@@ -1125,7 +1134,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
@@ -1136,7 +1145,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>39</v>
       </c>
@@ -1147,7 +1156,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
@@ -1158,7 +1167,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
@@ -1169,7 +1178,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
@@ -1180,7 +1189,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
@@ -1191,7 +1200,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
@@ -1202,7 +1211,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>45</v>
       </c>
@@ -1213,7 +1222,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>17</v>
       </c>
@@ -1224,7 +1233,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>15</v>
       </c>
@@ -1235,7 +1244,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>16</v>
       </c>
@@ -1246,7 +1255,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>3</v>
       </c>
@@ -1257,7 +1266,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>20</v>
       </c>
@@ -1268,7 +1277,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>46</v>
       </c>
@@ -1279,7 +1288,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>13</v>
       </c>
@@ -1290,7 +1299,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
@@ -1301,7 +1310,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>47</v>
       </c>
@@ -1312,7 +1321,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>48</v>
       </c>
@@ -1323,7 +1332,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>49</v>
       </c>
@@ -1334,7 +1343,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>50</v>
       </c>
@@ -1345,7 +1354,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>51</v>
       </c>
@@ -1356,7 +1365,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>52</v>
       </c>
@@ -1367,7 +1376,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>53</v>
       </c>
@@ -1378,7 +1387,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>54</v>
       </c>
@@ -1389,7 +1398,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>55</v>
       </c>
@@ -1400,7 +1409,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>56</v>
       </c>
@@ -1411,7 +1420,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>24</v>
       </c>
@@ -1422,7 +1431,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>23</v>
       </c>
@@ -1433,7 +1442,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>113</v>
       </c>
@@ -1444,7 +1453,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>115</v>
       </c>
@@ -1455,7 +1464,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>117</v>
       </c>
@@ -1466,7 +1475,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>119</v>
       </c>
@@ -1477,7 +1486,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>121</v>
       </c>
@@ -1488,7 +1497,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>123</v>
       </c>
@@ -1499,7 +1508,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>125</v>
       </c>
@@ -1510,7 +1519,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>127</v>
       </c>
@@ -1521,7 +1530,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>129</v>
       </c>
@@ -1532,7 +1541,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>131</v>
       </c>
@@ -1543,7 +1552,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>133</v>
       </c>
@@ -1554,7 +1563,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>135</v>
       </c>
@@ -1565,7 +1574,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>137</v>
       </c>
@@ -1574,6 +1583,28 @@
       </c>
       <c r="C68" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>139</v>
+      </c>
+      <c r="B69">
+        <v>500022150</v>
+      </c>
+      <c r="C69" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" t="s">
+        <v>141</v>
+      </c>
+      <c r="C70" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>